<commit_message>
emilia added EOD_report user story 27 Closing_The_Register user story 28 update_stock_with_sale func while making the sale update_sales  get_sales_report  user story 6
</commit_message>
<xml_diff>
--- a/workOnExcel/EOD.xlsx
+++ b/workOnExcel/EOD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="3">
   <si>
     <t>date</t>
   </si>
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -736,6 +736,22 @@
         <v>350</v>
       </c>
     </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>350</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>